<commit_message>
Update Widget Chat Ultra cool
</commit_message>
<xml_diff>
--- a/sessions.xlsx
+++ b/sessions.xlsx
@@ -448,13 +448,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="11.5703125" customWidth="1" min="1" max="1"/>
     <col width="38.42578125" customWidth="1" min="2" max="2"/>
@@ -802,6 +802,737 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>17</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: {'error': 'Your request has failed 4 retry attempts! Try clearing your chat history or make a ticket @ discord.gg/shuttleai including your model.', 'model': 'gpt-4'}
+role: user
+content: Привет
+role: assistant
+content: {'error': 'Your request has failed 4 retry attempts! Try clearing your chat history or make a ticket @ discord.gg/shuttleai including your model.', 'model': 'gpt-4'}
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>18</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: {'error': 'Model `gpt-3.5` not found! Try https://api.shuttleai.app/v1/models'}
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>19</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: {'choices': [{'finish_reason': 'stop', 'index': 0, 'message': {'content': 'Привет, как я могу помочь вам сегодня?', 'role': 'assistant'}}], 'created': 1703396009, 'id': 'chatcmpl-b4b533ec1f790f70fb73a62ea0150ab0', 'model': 'gpt-3.5-turbo', 'object': 'chat.completion', 'usage': {'completion_tokens': None, 'prompt_tokens': None, 'total_tokens': None}}
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>20</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: {'error': 'Your request has failed 4 retry attempts! Try clearing your chat history or make a ticket @ discord.gg/shuttleai including your model.', 'model': 'gpt-4'}
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>21</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Прив
+role: assistant
+content: {'choices': [{'finish_reason': 'stop', 'index': 0, 'message': {'content': 'Привет! Как я могу помочь вам сегодня?', 'role': 'assistant'}}], 'created': 1703396053, 'id': 'chatcmpl-a7188f0e3ee1cacca8f2127e0c8e370c', 'model': 'gpt-3.5-turbo', 'object': 'chat.completion', 'usage': {'completion_tokens': None, 'prompt_tokens': None, 'total_tokens': None}}
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>22</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Как я могу помочь вам сегодня?
+role: user
+content: Кто ты?
+role: assistant
+content: Я - нейропсихолог, готов помочь вам разгадать ваши внутренние проблемы и научиться справляться с ними.
+role: user
+content: У меня Депрессия
+role: assistant
+content: Какая жалость. Депрессия может быть очень тяжелым состоянием. Я готов помочь вам разобраться с этим и найти пути преодоления. Расскажите мне, что происходит у вас?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>23</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Прив
+role: assistant
+content: Привет! Как я могу помочь вам сегодня?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>24</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет, как я могу помочь вам сегодня?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>25</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Как я могу помочь вам сегодня?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>26</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет. Как я могу помочь вам сегодня?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>27</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Как я могу помочь вам сегодня?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>28</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Чем могу помочь?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>29</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Чем я могу помочь?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>30</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Как я могу помочь вам сегодня?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>31</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Как я могу помочь вам сегодня?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>32</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Как я могу помочь вам сегодня?
+role: user
+content: Кто ты?
+role: assistant
+content: Привет! Я нейропсихолог, готов помочь вам с вашей проблемой.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>33</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Как я могу помочь вам сегодня?
+role: user
+content: Кто ты?
+role: assistant
+content: Привет! Я нейропсихолог, готов помочь вам с вашей проблемой.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>34</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Как я могу помочь вам сегодня?
+role: user
+content: Кто ты и зачем?
+role: assistant
+content: Я - нейропсихолог, готов помочь вам разобраться с вашими проблемами и состоянием. Как я могу помочь вам сегодня?
+role: user
+content: Расскажи о суициде
+role: assistant
+content: Как нейропсихолог, моя задача помочь вам разобраться с вашими проблемами и состоянием. Расскажите, что вас беспокоит по этому поводу?
+role: user
+content: У меня Депрессия
+role: assistant
+content: Как нейропсихолог, моя задача помочь вам разобраться с вашими проблемами и состоянием. Расскажите, что вас беспокоит по этому поводу?
+role: user
+content: Меня обижают((
+role: assistant
+content: Как нейропсихолог, моя задача помочь вам разобраться с вашими проблемами и состоянием. Расскажите подробнее о ситуации, которая вызывает у вас чувство обиды.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>35</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Как я могу помочь вам сегодня?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>36</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Как я могу помочь вам сегодня?
+role: user
+content: Кто ты и зачем?
+role: assistant
+content: Я - психолог, готов помочь вам разобраться с вашими проблемами. Если у вас есть какие-то затруднения или нужно обсудить что-то, я тут для вас.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>37</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Как я могу помочь вам сегодня?
+role: user
+content: Кто ты?
+role: assistant
+content: Я нейропсихолог и готов помочь вам разобраться с любыми вопросами или трудностями, связанными с вашим психическим состоянием. Чем я могу помочь?
+role: user
+content: У меня депрессия
+role: assistant
+content: Понимаю, что депрессия может быть трудным периодом. Я готов вас выслушать. Расскажите мне больше о том, что вы чувствуете, и мы вместе постараемся найти пути к облегчению вашего состояния.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>38</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Как я могу помочь вам сегодня?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>39</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Как я могу вам помочь сегодня?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>40</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Как я могу помочь вам сегодня?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>41</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Как я могу помочь вам сегодня?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>42</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Как я могу помочь вам сегодня?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>43</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Как я могу помочь вам сегодня?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>44</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Как я могу помочь вам сегодня?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>45</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Как я могу помочь вам сегодня?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>46</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Как я могу помочь вам сегодня?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>47</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Как я могу помочь вам сегодня?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>48</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Как я могу помочь вам сегодня?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>49</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: tyrghrtytry
+role: assistant
+content: Привет! Похоже, ваш вопрос не совсем понятен. Если у вас есть конкретная проблема или вопрос, с которым вы хотели бы обратиться за помощью, пожалуйста, опишите ее более подробно. Я здесь, чтобы помочь вам с психологическими вопросами и трудностями.
+</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+score: Хорошо
+comment: Хорошо, 
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>50</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Как я могу помочь вам сегодня?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>51</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Как я могу помочь вам сегодня?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>52</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Как я могу помочь вам сегодня?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>53</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Как я могу помочь вам сегодня?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>54</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Здравствуйте! Как я могу помочь вам сегодня?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>55</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Как я могу помочь вам сегодня?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>56</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Как я могу помочь вам сегодня?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>57</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Как я могу помочь вам сегодня?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>58</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Как я могу помочь вам сегодня?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>59</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: ыы
+role: assistant
+content: Привет! Как я могу помочь тебе сегодня? Если у тебя есть какие-то вопросы или заботы, не стесняйся поделиться ими.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>60</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привет
+role: assistant
+content: Привет! Как я могу помочь?
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>61</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+role: user
+content: Привкт\
+role: assistant
+content: Привет! Как я могу помочь вам сегодня?
+</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>